<commit_message>
Added Chamber fan to the BOM
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/Valkyrie BOM v1.0.0.xlsx
+++ b/Document Library/Bill Of Materials/Valkyrie BOM v1.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="560" documentId="11_BB46956AE7341EA83D7747123DA4EA88538076BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EB1C4C1-7E99-4374-965D-0B524BC889FF}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="11_BB46956AE7341EA83D7747123DA4EA88538076BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{836CD9A1-9054-41AE-A2CE-B0F57FAA0897}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1517,10 +1517,10 @@
     <t>1 x 20 PCs M4 x 50 SS</t>
   </si>
   <si>
-    <t>1x Sunon MB60252VX</t>
-  </si>
-  <si>
-    <t>60mm Sunon MB60252VX</t>
+    <t>60mm Sunon MF60202V3</t>
+  </si>
+  <si>
+    <t>1x Sunon MF60202V3</t>
   </si>
 </sst>
 </file>
@@ -3239,7 +3239,7 @@
       <c r="H2" s="45"/>
       <c r="I2" s="46">
         <f>I60</f>
-        <v>1872.1400000000003</v>
+        <v>1887.6400000000003</v>
       </c>
       <c r="J2" s="44"/>
       <c r="K2" s="51"/>
@@ -5031,7 +5031,7 @@
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B51" t="s">
         <v>111</v>
@@ -5040,23 +5040,23 @@
         <v>158</v>
       </c>
       <c r="D51" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F51" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G51" s="10">
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="H51" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I51" s="40">
         <f t="shared" si="2"/>
-        <v>8.5</v>
+        <v>24</v>
       </c>
       <c r="J51" s="115" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="K51" s="12" t="s">
         <v>185</v>
@@ -5362,7 +5362,7 @@
       <c r="H60" s="45"/>
       <c r="I60" s="46">
         <f>SUM(I20:I59)+I14</f>
-        <v>1872.1400000000003</v>
+        <v>1887.6400000000003</v>
       </c>
       <c r="J60" s="44"/>
       <c r="K60" s="51"/>
@@ -5401,7 +5401,7 @@
     <hyperlink ref="J44" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="J45" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="J50" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="J51" r:id="rId23" display="1x Size: NEW" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="J51" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="J52" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="J53" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="J32" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>

</xml_diff>